<commit_message>
20200830: Set ghosts, packman automovement
</commit_message>
<xml_diff>
--- a/Maps/createMap.xlsx
+++ b/Maps/createMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\packman\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7D170E-F4F4-48F9-9911-7107E23E20C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF36ED3-0D47-43A4-81FD-E2CD8E2C0F75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F00F83BC-96EA-406B-B90B-F4DE5BA56F0D}"/>
   </bookViews>
@@ -34,8 +34,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -63,33 +71,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -107,16 +96,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -440,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB2D831-4F7A-4F53-BECF-2FBB20E76F1D}">
-  <dimension ref="A1:X12"/>
+  <dimension ref="A1:X16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,81 +432,81 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -536,58 +515,58 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V2">
         <v>0</v>
@@ -596,335 +575,335 @@
         <v>0</v>
       </c>
       <c r="X2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W3">
         <v>0</v>
       </c>
       <c r="X3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K7">
         <v>3</v>
@@ -936,264 +915,264 @@
         <v>3</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="N10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W10">
         <v>0</v>
       </c>
       <c r="X10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1202,58 +1181,58 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
       <c r="N11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V11">
         <v>0</v>
@@ -1262,95 +1241,99 @@
         <v>0</v>
       </c>
       <c r="X11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X12">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="H16" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:X12">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>